<commit_message>
Updated Immobilienliste via Workflow
</commit_message>
<xml_diff>
--- a/Immobilienliste.xlsx
+++ b/Immobilienliste.xlsx
@@ -478,37 +478,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Wolfgang Schweidler</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Wohnung in St. Gallen</t>
+          <t>Top of St. Gallen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Wohnung • 4.5 Zi. • 94 m²</t>
+          <t>Wohnung • 6 Zi. • 170 m²</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Wohnung • 4.5 Zi. • 94 m²</t>
+          <t>Wohnung • 6 Zi. • 170 m²</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CHF 2’050.</t>
+          <t>CHF 3’230.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CHF 262</t>
+          <t>CHF 228</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Gesstreppe 1, 9011 St. Gallen</t>
+          <t>Reherstrasse 20c, 9016 St. Gallen</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -523,30 +523,34 @@
           <t>—</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Helle Altbau 3-Zimmerwohnung</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 53 m²</t>
+          <t>Wohnung • 3 Zi. • 90 m²</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 53 m²</t>
+          <t>Wohnung • 3 Zi. • 90 m²</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CHF 1’150.</t>
+          <t>CHF 1’300.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CHF 260</t>
+          <t>CHF 173</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>9015 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -563,32 +567,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gepflegte schöne 3 1/2 Zimmer-Dachwohnung</t>
+          <t>Zentrale 3.5 Zi-Whg mit Balkon</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Wohnung • 3.5 Zi. • 74 m²</t>
+          <t>Wohnung • 3.5 Zi.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Wohnung • 3.5 Zi. • 74 m²</t>
+          <t>Wohnung • 3.5 Zi.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CHF 1’490.</t>
+          <t>CHF 1’140.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>CHF 242</t>
+          <t>—</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9008 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -605,27 +609,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5 ½-Zimmer-Wohnung im Museumsquartier</t>
+          <t>2 in 1 Room for Rent</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 135 m²</t>
+          <t>Wohnung • 5 Zi.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 135 m²</t>
+          <t>Wohnung • 5 Zi.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CHF 2’780.</t>
+          <t>CHF 605.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CHF 247</t>
+          <t>—</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -662,12 +666,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CHF 1’750.</t>
+          <t>CHF 1’875.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CHF 300</t>
+          <t>CHF 321</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -684,359 +688,359 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GEMAG Gebrüder Müller AG</t>
+          <t>—</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Stilvolle Wohnung in Gehdistanz zum Stadtzentrum</t>
+          <t>Wohnung in St. Gallen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 75 m²</t>
+          <t>Wohnung • 4.5 Zi. • 94 m²</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 75 m²</t>
+          <t>Wohnung • 4.5 Zi. • 94 m²</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CHF 1’485.</t>
+          <t>CHF 2’050.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CHF 238</t>
+          <t>CHF 262</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9000 St. Gallen</t>
+          <t>Gesstreppe 1, 9011 St. Gallen</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>flatfox.ch</t>
+          <t>immoscout24.ch</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sproll &amp; Ramseyer AG</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2.5 Zimmerwohnung direkt an der Uni</t>
-        </is>
-      </c>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 49 m²</t>
+          <t>Wohnung • 2.5 Zi. • 53 m²</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 49 m²</t>
+          <t>Wohnung • 2.5 Zi. • 53 m²</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CHF 1’430.</t>
+          <t>CHF 1’150.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>CHF 350</t>
+          <t>CHF 260</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Höhenweg 13, 9000 St. Gallen</t>
+          <t>9015 St. Gallen</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>newhome.ch</t>
+          <t>flatfox.ch</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Salina ProImmo AG</t>
+          <t>—</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Charmantes Dach-Studio in Zentrumsnähe</t>
+          <t>gepflegte schöne 3 1/2 Zimmer-Dachwohnung</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Penthouse • 1.5 Zi.</t>
+          <t>Wohnung • 3.5 Zi. • 74 m²</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Penthouse • 1.5 Zi.</t>
+          <t>Wohnung • 3.5 Zi. • 74 m²</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CHF 670.</t>
+          <t>CHF 1’490.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>CHF 242</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9000 St. Gallen</t>
+          <t>9008 St. Gallen</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>newhome.ch</t>
+          <t>flatfox.ch</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>—</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Liebhaberobjekt: Absolute Alleinlage</t>
+          <t>5 ½-Zimmer-Wohnung im Museumsquartier</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Einfamilienhaus • 3.5 Zi.</t>
+          <t>Wohnung • 5.5 Zi. • 135 m²</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Einfamilienhaus • 3.5 Zi.</t>
+          <t>Wohnung • 5.5 Zi. • 135 m²</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Auf Anfrage</t>
+          <t>CHF 2’780.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>CHF 247</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>9011 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>immoscout24.ch</t>
+          <t>flatfox.ch</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EIKO Verwaltungs AG</t>
+          <t>UMS AG - Untermietservice - Temporary Housing</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>helle 4.5-Zimmerwohnung an ruhiger Lage</t>
+          <t>3 ZI-WOHNUNG IN ST. GALLEN - ST. GEORGEN, MÖBLIERT, TEMPORÄR</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Terrassenwohnung • 4.5 Zi. • 115 m²</t>
+          <t>Möblierte Wohnung • 3 Zi. • 70 m²</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Terrassenwohnung • 4.5 Zi. • 115 m²</t>
+          <t>Möblierte Wohnung • 3 Zi. • 70 m²</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CHF 2’730.</t>
+          <t>CHF 1’750.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>CHF 285</t>
+          <t>CHF 300</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>9011 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>immoscout24.ch</t>
+          <t>homegate.ch</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HN Verwaltungs GmbH</t>
+          <t>Sproll &amp; Ramseyer AG</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Zentral im Herzen von SG, renovierte Dachgeschosswohnung</t>
+          <t>2.5 Zimmerwohnung direkt an der Uni</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Penthouse • 2 Zi. • 35 m²</t>
+          <t>Wohnung • 2.5 Zi. • 49 m²</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Penthouse • 2 Zi. • 35 m²</t>
+          <t>Wohnung • 2.5 Zi. • 49 m²</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CHF 930.</t>
+          <t>CHF 1’430.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>CHF 319</t>
+          <t>CHF 350</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Linsebühlstrasse 92, 9000 St. Gallen</t>
+          <t>Höhenweg 13, 9000 St. Gallen</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>immoscout24.ch</t>
+          <t>newhome.ch</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>aro immo ag</t>
+          <t>EIKO Verwaltungs AG</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Moderne 5 ½-Zimmer Maisonette-Wohnung an ruhiger, zentraler Lage</t>
+          <t>helle 4.5-Zimmerwohnung an ruhiger Lage</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 170 m²</t>
+          <t>Terrassenwohnung • 4.5 Zi. • 115 m²</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 170 m²</t>
+          <t>Terrassenwohnung • 4.5 Zi. • 115 m²</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CHF 2’710.</t>
+          <t>CHF 2’730.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CHF 191</t>
+          <t>CHF 285</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>9000 St. Gallen</t>
+          <t>9011 St. Gallen</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>icasa.ch</t>
+          <t>immoscout24.ch</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>HN Verwaltungs GmbH</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Zentral im Herzen von SG, renovierte Dachgeschosswohnung</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 45 m²</t>
+          <t>Penthouse • 2 Zi. • 35 m²</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 45 m²</t>
+          <t>Penthouse • 2 Zi. • 35 m²</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CHF 960.</t>
+          <t>CHF 930.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>CHF 256</t>
+          <t>CHF 319</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>9016 St. Gallen</t>
+          <t>Linsebühlstrasse 92, 9000 St. Gallen</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>flatfox.ch</t>
+          <t>immoscout24.ch</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Dave</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Grosse helle Wohnung in St. Gallen</t>
+          <t>Liebhaberobjekt: Absolute Alleinlage</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi.</t>
+          <t>Einfamilienhaus • 3.5 Zi.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi.</t>
+          <t>Einfamilienhaus • 3.5 Zi.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CHF 2’375.</t>
+          <t>Auf Anfrage</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1046,44 +1050,44 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>9000 St. Gallen</t>
+          <t>9011 St. Gallen</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>flatfox.ch</t>
+          <t>homegate.ch</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IDP Treuhand AG</t>
+          <t>aro immo ag</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>gemütliche Wohnung an ruhiger Lage</t>
+          <t>Moderne 5 ½-Zimmer Maisonette-Wohnung an ruhiger, zentraler Lage</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 40 m²</t>
+          <t>Wohnung • 5.5 Zi. • 170 m²</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 40 m²</t>
+          <t>Wohnung • 5.5 Zi. • 170 m²</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CHF 800.</t>
+          <t>CHF 2’710.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>CHF 240</t>
+          <t>CHF 191</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1093,81 +1097,77 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>newhome.ch</t>
+          <t>icasa.ch</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Die Immo AG</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Grosszügige 2.5 Zimmer Neubau Wohnung St. Gallen - St. Fiden</t>
-        </is>
-      </c>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 68 m²</t>
+          <t>Wohnung • 2 Zi. • 45 m²</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 68 m²</t>
+          <t>Wohnung • 2 Zi. • 45 m²</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CHF 1’770.</t>
+          <t>CHF 960.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>CHF 315</t>
+          <t>CHF 256</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>9000 St. Gallen</t>
+          <t>9016 St. Gallen</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>newhome.ch</t>
+          <t>flatfox.ch</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>St.Galler Pensionskasse</t>
+          <t>—</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Die nette Kleinwohnung im Hochparterre</t>
+          <t>Grosse helle Wohnung in St. Gallen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 49 m²</t>
+          <t>Wohnung • 5.5 Zi.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Wohnung • 2 Zi. • 49 m²</t>
+          <t>Wohnung • 5.5 Zi.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CHF 1’020.</t>
+          <t>CHF 2’375.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>CHF 250</t>
+          <t>—</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1177,34 +1177,34 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>homegate.ch</t>
+          <t>flatfox.ch</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>St.Galler Pensionskasse</t>
+          <t>IDP Treuhand AG</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kleinwohnung an bester Lage</t>
+          <t>gemütliche Wohnung an ruhiger Lage</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Wohnung • 3 Zi. • 61 m²</t>
+          <t>Wohnung • 2 Zi. • 40 m²</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Wohnung • 3 Zi. • 61 m²</t>
+          <t>Wohnung • 2 Zi. • 40 m²</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CHF 1’220.</t>
+          <t>CHF 800.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1219,39 +1219,39 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>homegate.ch</t>
+          <t>newhome.ch</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>Die Immo AG</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3.5-Zimmer, 83 m², Dachgeschosswohnung</t>
+          <t>Grosszügige 2.5 Zimmer Neubau Wohnung St. Gallen - St. Fiden</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Penthouse • 3.5 Zi. • 83 m²</t>
+          <t>Wohnung • 2.5 Zi. • 68 m²</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Penthouse • 3.5 Zi. • 83 m²</t>
+          <t>Wohnung • 2.5 Zi. • 68 m²</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CHF 1’580.</t>
+          <t>CHF 1’770.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>CHF 228</t>
+          <t>CHF 315</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1268,37 +1268,37 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Galli Immo-Service AG</t>
+          <t>St.Galler Pensionskasse</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ruhige Familien-Stadtwohnung in St. Fiden</t>
+          <t>Die nette Kleinwohnung im Hochparterre</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Wohnung • 4.5 Zi. • 80 m²</t>
+          <t>Wohnung • 2 Zi. • 49 m²</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Wohnung • 4.5 Zi. • 80 m²</t>
+          <t>Wohnung • 2 Zi. • 49 m²</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CHF 1’390.</t>
+          <t>CHF 1’020.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>CHF 209</t>
+          <t>CHF 250</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Helvetiastrasse 33, 9000 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1310,121 +1310,121 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Liegenschaften Treuhand St.Gallen AG</t>
+          <t>St.Galler Pensionskasse</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>repräsentative 5,5 Zimmer-Wohnung am Fusse des Rosenberges</t>
+          <t>Kleinwohnung an bester Lage</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 151 m²</t>
+          <t>Wohnung • 3 Zi. • 61 m²</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Wohnung • 5.5 Zi. • 151 m²</t>
+          <t>Wohnung • 3 Zi. • 61 m²</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CHF 2’934.</t>
+          <t>CHF 1’220.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>CHF 233</t>
+          <t>CHF 240</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Greifenstrasse 17, 9000 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>immoscout24.ch</t>
+          <t>homegate.ch</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Max Pfister Baubüro AG</t>
+          <t>—</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3.5-Zimmerwohnung im 2. Stock</t>
+          <t>3.5-Zimmer, 83 m², Dachgeschosswohnung</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Wohnung • 3.5 Zi.</t>
+          <t>Penthouse • 3.5 Zi. • 83 m²</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Wohnung • 3.5 Zi.</t>
+          <t>Penthouse • 3.5 Zi. • 83 m²</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CHF 1’435.</t>
+          <t>CHF 1’580.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>CHF 228</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Reherstrasse 14a, 9016 St. Gallen</t>
+          <t>9000 St. Gallen</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>immoscout24.ch</t>
+          <t>newhome.ch</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>VTAG Verwaltungs- und Treuhand AG</t>
+          <t>Galli Immo-Service AG</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Schöne Erdgeschoss Wohnung mit Gartensitzplatz</t>
+          <t>Ruhige Familien-Stadtwohnung in St. Fiden</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Wohnung • 3 Zi. • 68 m²</t>
+          <t>Wohnung • 4.5 Zi. • 80 m²</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Wohnung • 3 Zi. • 68 m²</t>
+          <t>Wohnung • 4.5 Zi. • 80 m²</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CHF 1’490.</t>
+          <t>CHF 1’390.</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CHF 263</t>
+          <t>CHF 209</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>9008 St. Gallen</t>
+          <t>Helvetiastrasse 33, 9000 St. Gallen</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1436,42 +1436,42 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Crowdhouse AG</t>
+          <t>Liegenschaften Treuhand St.Gallen AG</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>WOHNEN MIT AUSSICHT</t>
+          <t>repräsentative 1.5 Zimmer-Wohnung am Fusse des Rosenberges</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 51 m²</t>
+          <t>Wohnung • 5.5 Zi. • 151 m²</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Wohnung • 2.5 Zi. • 51 m²</t>
+          <t>Wohnung • 5.5 Zi. • 151 m²</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CHF 1’320.</t>
+          <t>CHF 2’934.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CHF 311</t>
+          <t>CHF 233</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>9008 St. Gallen</t>
+          <t>Greifenstrasse 17, 9000 St. Gallen</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>homegate.ch</t>
+          <t>immoscout24.ch</t>
         </is>
       </c>
     </row>

</xml_diff>